<commit_message>
Update Lab 1 Expected Results Table and register_test.sv for better clarity
</commit_message>
<xml_diff>
--- a/tables/Lab1_ExpectedResultsTable.xlsx
+++ b/tables/Lab1_ExpectedResultsTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\potterst\Documents\CompOrg\Fall_2020\Lab\ARM-Lab_Fall_2020\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94262F05-F56A-435D-B583-D91496B888D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DD5309-BAF5-4035-B8CC-838EF2E4825B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{2EEAC87F-AC07-4F0F-96B3-36AE6E943B68}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{2EEAC87F-AC07-4F0F-96B3-36AE6E943B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,22 +791,22 @@
         <v>5</v>
       </c>
       <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <v>527</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>-8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>77</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>4</v>
-      </c>
-      <c r="G4" s="1">
-        <v>18</v>
       </c>
       <c r="H4" s="1">
         <v>18</v>
@@ -860,8 +860,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="D4" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add update times to Lab 1 Expected Results Tables
</commit_message>
<xml_diff>
--- a/tables/Lab1_ExpectedResultsTable.xlsx
+++ b/tables/Lab1_ExpectedResultsTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\potterst\Documents\CompOrg\Fall_2020\Lab\ARM-Lab_Fall_2020\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven_p_potter\Box\ELC3338\Fall2021_test\ARM-Lab\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DD5309-BAF5-4035-B8CC-838EF2E4825B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB5AE48-0203-4EEC-9EF7-ADBA422DB7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{2EEAC87F-AC07-4F0F-96B3-36AE6E943B68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{2EEAC87F-AC07-4F0F-96B3-36AE6E943B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Test Case</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>3771334343958392850</t>
+  </si>
+  <si>
+    <t>d update time</t>
+  </si>
+  <si>
+    <t>rst update time</t>
   </si>
 </sst>
 </file>
@@ -299,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -316,6 +322,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,7 +645,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,6 +861,70 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="17">
+        <v>0</v>
+      </c>
+      <c r="C6" s="16">
+        <v>10</v>
+      </c>
+      <c r="D6" s="16">
+        <v>20</v>
+      </c>
+      <c r="E6" s="16">
+        <v>30</v>
+      </c>
+      <c r="F6" s="16">
+        <v>40</v>
+      </c>
+      <c r="G6" s="16">
+        <v>50</v>
+      </c>
+      <c r="H6" s="16">
+        <v>52</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="16">
+        <v>69</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="16">
+        <v>87</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1">
+        <v>63</v>
+      </c>
+      <c r="J7" s="1">
+        <v>69</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
+        <v>80</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
+        <v>89</v>
+      </c>
+      <c r="O7" s="1"/>
+    </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
@@ -859,6 +932,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="71" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="71" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>